<commit_message>
fehler, prioritäten, status, tracker, umgebung hinzugefügt
</commit_message>
<xml_diff>
--- a/Aufgaben/Aufgabenblatt1/Aufgabe1.xlsx
+++ b/Aufgaben/Aufgabenblatt1/Aufgabe1.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Documents\HS_RM\Workspaces\Softwaretesting\Aufgaben\Aufgabenblatt1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Documents\HS_RM\Workspaces\STesting\Aufgaben\Aufgabenblatt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717F1570-0CAA-4B4D-B463-E158B63589DE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932AEBF-62A5-451A-B020-53269830AA43}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fehlerbeschreibung" sheetId="1" r:id="rId1"/>
-    <sheet name="Fehlerlebenszyklus" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hilfstabelle" sheetId="4" r:id="rId2"/>
+    <sheet name="Fehlerlebenszyklus" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Priority">Fehlerbeschreibung!$C$45:$C$47</definedName>
-    <definedName name="Serverity">Fehlerbeschreibung!$B$45:$B$48</definedName>
+    <definedName name="Priority">Fehlerbeschreibung!$C$51:$C$53</definedName>
+    <definedName name="Serverity">Fehlerbeschreibung!$B$52:$B$55</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>ID:</t>
   </si>
@@ -92,12 +99,123 @@
   </si>
   <si>
     <t>Geschlossen</t>
+  </si>
+  <si>
+    <t>Produktiv</t>
+  </si>
+  <si>
+    <t>Analysieren</t>
+  </si>
+  <si>
+    <t>Vorbereiten</t>
+  </si>
+  <si>
+    <t>Testen</t>
+  </si>
+  <si>
+    <t>TL Ok</t>
+  </si>
+  <si>
+    <t>TL Abbruch</t>
+  </si>
+  <si>
+    <t>TL Abweichung</t>
+  </si>
+  <si>
+    <t>Warten</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Fehler</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Unterstützung</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Tracker:</t>
+  </si>
+  <si>
+    <t>Tracker</t>
+  </si>
+  <si>
+    <t>Anforderung</t>
+  </si>
+  <si>
+    <t>Aufgabe</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Kategorie:</t>
+  </si>
+  <si>
+    <t>Niedrig</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Hoch</t>
+  </si>
+  <si>
+    <t>Dringend</t>
+  </si>
+  <si>
+    <t>Sofort</t>
+  </si>
+  <si>
+    <t>Kunde</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>Plattform:</t>
+  </si>
+  <si>
+    <t>Abgwiesen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -191,9 +309,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -203,6 +318,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -541,66 +661,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showFormulas="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
@@ -616,17 +743,23 @@
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="D9" s="8" t="s">
         <v>8</v>
       </c>
@@ -641,18 +774,18 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="2:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
@@ -662,48 +795,12 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C2:E2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C12:E12"/>
@@ -723,11 +820,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ungültiger Status" error="Wählen Sie einen Status aus der Liste aus." promptTitle="Status" prompt="Wählen Sie einen Status aus der Liste aus." sqref="C5" xr:uid="{5ED33D8D-2986-4306-AF63-6696BAE2DD2E}">
-      <formula1>$B$23:$B$29</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -750,30 +842,285 @@
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ungültiger Status" error="Wählen Sie einen Status aus der Liste aus." promptTitle="Status" prompt="Wählen Sie einen Status aus der Liste aus." xr:uid="{5ED33D8D-2986-4306-AF63-6696BAE2DD2E}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$A$3:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ungültiger Tracker" error="Bitte einen Tracker aus der Liste auswählen" promptTitle="Tracker eingeben" prompt="Bitte einen Tracker aus der Liste auswählen" xr:uid="{646B1F4B-661D-4979-8A2D-9455A1651FFB}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$C$3:$C$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Gültige Kategorie auswählen" error="Bitte eine gültige Kategorie aus der Liste auswählen" promptTitle="Kategorie eingeben" prompt="Bitte Kategorie aus der Liste auswählen" xr:uid="{86EFEA87-9090-495E-B277-E0B7127D55D1}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$E$3:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Gültige Priorität auswählen" error="Bitte gültige Priorität aus der Liste auswählen" promptTitle="Priorität auswählen" prompt="Priorität aus der Liste auswählen" xr:uid="{CA7C5E37-B9BC-4141-AB29-AD89890FA29F}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$G$3:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ungültige Plattform" error="Bitte gültige Plattform aus der Liste auswählen" promptTitle="Plattform auswählen" prompt="Bitte Plattform auswählen" xr:uid="{C0C57CB1-BF79-48FE-B9F6-39523F7BBB60}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$I$3:$I$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6097B94-F70E-43DD-B130-B41690572E02}">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B8:T22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+      <c r="R11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>